<commit_message>
changes for cash invoice generation
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-Cash-v1.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-Cash-v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/aroundlocalhost/application/controllers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-dev/application/controllers/excel-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$10:$J$11</definedName>
-    <definedName name="booking_details__9" localSheetId="0">Sheet1!$B$10:$J$11</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$J$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$11:$I$12</definedName>
+    <definedName name="booking_details__9" localSheetId="0">Sheet1!$B$11:$I$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$I$26</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -54,14 +54,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Booking ID</t>
   </si>
   <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
     <t>Closed Date</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>{booking:service_name}</t>
   </si>
   <si>
-    <t>{booking:booking_date}</t>
-  </si>
-  <si>
     <t>{booking:closed_date}</t>
   </si>
   <si>
@@ -188,10 +182,31 @@
     <t>Invoice Number: {meta:invoice_id}</t>
   </si>
   <si>
-    <t>Invoice Period: {meta:sd} TO {meta:ed}</t>
-  </si>
-  <si>
     <t>Bookings: {meta:count}</t>
+  </si>
+  <si>
+    <t>Add. Service Charge</t>
+  </si>
+  <si>
+    <t>Period: {meta:sd} TO {meta:ed}</t>
+  </si>
+  <si>
+    <t>{meta:t_ap}</t>
+  </si>
+  <si>
+    <t>{meta:r_sc}</t>
+  </si>
+  <si>
+    <t>{meta:r_asc}</t>
+  </si>
+  <si>
+    <t>{meta:r_pc}</t>
+  </si>
+  <si>
+    <t>{meta:r_total}</t>
+  </si>
+  <si>
+    <t>{meta:msg}</t>
   </si>
 </sst>
 </file>
@@ -690,11 +705,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -702,9 +714,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,9 +750,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -792,12 +798,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,7 +831,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -850,8 +849,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -927,13 +935,13 @@
     <xf numFmtId="1" fontId="5" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -964,15 +972,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>116254</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>51777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>192457</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>9769</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1276,236 +1284,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="0.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="47" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="47" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="4" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="7" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5.1640625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="1.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="42" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="42" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="7" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.83203125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="12" x14ac:dyDescent="0.15">
-      <c r="B1" s="1"/>
-      <c r="C1" s="48" t="s">
+    <row r="1" spans="1:9" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" ht="12" x14ac:dyDescent="0.2">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
+    </row>
+    <row r="3" spans="1:9" ht="12" x14ac:dyDescent="0.15">
+      <c r="B3" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="12" x14ac:dyDescent="0.15">
+      <c r="B4" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="12" x14ac:dyDescent="0.15">
+      <c r="B5" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="12" x14ac:dyDescent="0.15">
+      <c r="B6" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="12" x14ac:dyDescent="0.15">
+      <c r="B7" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="12" x14ac:dyDescent="0.15">
+      <c r="B8" s="46"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="12" x14ac:dyDescent="0.15">
+      <c r="B9" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" s="16" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
-    </row>
-    <row r="2" spans="2:10" ht="12" x14ac:dyDescent="0.15">
-      <c r="B2" s="5"/>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="2:10" ht="12" x14ac:dyDescent="0.15">
-      <c r="B3" s="5"/>
-      <c r="C3" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="2:10" ht="12" x14ac:dyDescent="0.15">
-      <c r="B4" s="5"/>
-      <c r="C4" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="2:10" ht="12" x14ac:dyDescent="0.15">
-      <c r="B5" s="5"/>
-      <c r="C5" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="2:10" ht="12" x14ac:dyDescent="0.15">
-      <c r="B6" s="5"/>
-      <c r="C6" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="2:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="2:10" ht="12" x14ac:dyDescent="0.15">
-      <c r="B8" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
-      <c r="C9" s="56" t="s">
+      <c r="G11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="B12" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="2:10" s="19" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="16" t="s">
+    </row>
+    <row r="13" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="63" t="s">
         <v>8</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="B11" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="68"/>
-    </row>
-    <row r="14" spans="2:10" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="63" t="e">
-        <f>"Thanks 247around partner for your support, we completed {meta:count} bookings with you from {meta:sd} till {meta:ed}, total transaction value for the bookings was Rs. " &amp; I16 &amp;  ". Around royalty for this invoice is Rs. " &amp; G19 &amp; ". Your rating for completed bookings is " &amp; J16 &amp; ". We look forward to your continued support in future. As a next step, please make the final amount transfer as per below details."</f>
-        <v>#VALUE!</v>
       </c>
       <c r="C14" s="64"/>
       <c r="D14" s="64"/>
@@ -1513,211 +1487,206 @@
       <c r="F14" s="64"/>
       <c r="G14" s="64"/>
       <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="65"/>
-    </row>
-    <row r="15" spans="2:10" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="79"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="25" t="s">
+      <c r="I14" s="65"/>
+    </row>
+    <row r="15" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="62"/>
+    </row>
+    <row r="16" spans="1:9" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="76"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="37" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="75"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29" t="s">
+      <c r="H16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="37" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="72"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="H17" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="29">
-        <f>SUM(F16:H16)</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="75" t="s">
+    </row>
+    <row r="18" spans="2:9" ht="13" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="73"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="28">
+        <v>0.3</v>
+      </c>
+      <c r="F18" s="28">
+        <v>0.15</v>
+      </c>
+      <c r="G18" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="2:9" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="73"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" spans="2:9" ht="13" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="31">
-        <v>0.3</v>
-      </c>
-      <c r="G17" s="31">
-        <v>0.15</v>
-      </c>
-      <c r="H17" s="32">
-        <v>0.05</v>
-      </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-    </row>
-    <row r="18" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="75" t="s">
+      <c r="C20" s="75"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="35"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
+    </row>
+    <row r="21" spans="2:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="2:9" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="81"/>
+    </row>
+    <row r="23" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+      <c r="B23" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="67"/>
+      <c r="D23" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="84"/>
+    </row>
+    <row r="24" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+      <c r="B24" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="69"/>
+      <c r="D24" s="54">
+        <v>102405500277</v>
+      </c>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="56"/>
+    </row>
+    <row r="25" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+      <c r="B25" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="69"/>
+      <c r="D25" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="56"/>
+    </row>
+    <row r="26" spans="2:9" ht="13" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="35" t="e">
-        <f>F16*0.3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" s="35" t="e">
-        <f>G16*0.15</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H18" s="36" t="e">
-        <f>H16*0.05</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
-    </row>
-    <row r="19" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="77" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39" t="e">
-        <f>ROUND((SUM(F18:H18)),0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="42"/>
-    </row>
-    <row r="20" spans="2:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="46"/>
-    </row>
-    <row r="21" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="82" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="84"/>
-    </row>
-    <row r="22" spans="2:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="B22" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="85" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="87"/>
-    </row>
-    <row r="23" spans="2:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="B23" s="71" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="57">
-        <v>102405500277</v>
-      </c>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="59"/>
-    </row>
-    <row r="24" spans="2:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="B24" s="71" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="59"/>
-    </row>
-    <row r="25" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="73" t="s">
+      <c r="C26" s="71"/>
+      <c r="D26" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="62"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D24:I24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>